<commit_message>
Thread test & Annotation check
</commit_message>
<xml_diff>
--- a/findbyfilewebelement/src/test/resources/excel/ThreadPOExcelOneData.xlsx
+++ b/findbyfilewebelement/src/test/resources/excel/ThreadPOExcelOneData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2190" windowWidth="14220" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2190" windowWidth="14670" windowHeight="6750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:G21"/>
 </workbook>
 </file>
 
@@ -34,13 +33,13 @@
     <t>Class</t>
   </si>
   <si>
-    <t>file.pagefactory.MultipleThreadCacheTest$PageObjectExcelFirst</t>
-  </si>
-  <si>
     <t>element1</t>
   </si>
   <si>
     <t>element2</t>
+  </si>
+  <si>
+    <t>file.pagefactory.excel.ExcelFPMultipleThreadCacheTest$PageObjectExcelFirst</t>
   </si>
 </sst>
 </file>
@@ -387,12 +386,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -414,30 +413,30 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>